<commit_message>
added training and coursework information
</commit_message>
<xml_diff>
--- a/khurana_cv/data/cv_entries.xlsx
+++ b/khurana_cv/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDXC\University of Oregon Dropbox\Havi Khurana\Personal\Coding projects\khurana_cv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D678FA-F544-4604-BC4C-C0E5F234084E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E62DDE7-A363-4DAA-8CFD-F345B87F1DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,6 +196,85 @@
     <t>300</t>
   </si>
   <si>
+    <t>College of Education</t>
+  </si>
+  <si>
+    <t>7000</t>
+  </si>
+  <si>
+    <t>Ph.D. Quantitative Research Methods in Education</t>
+  </si>
+  <si>
+    <t>For presenting research at AEFP, Baltimore, 2023</t>
+  </si>
+  <si>
+    <t>For attending workshop on 'Big Data with Arrow in R' at PostIt, Seattle, 2024</t>
+  </si>
+  <si>
+    <t>For poster titled Who Are the Students Schools Frequently Suspend?</t>
+  </si>
+  <si>
+    <t>For poster titled Diversity, Expenditure, and Achievement in US Public Schools</t>
+  </si>
+  <si>
+    <t>Summer 2022-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked with Dr. David Liebowitz on projects related to school leadership and school discipline
+</t>
+  </si>
+  <si>
+    <t>Worked with Dr. Gina Biancarosa and Dr. Patrick Kennedy on projects related to Dynamic Indicators of Basic Early Literacy Skill (DIBELS8) reading assessments</t>
+  </si>
+  <si>
+    <t>Research Contract</t>
+  </si>
+  <si>
+    <t>Edunomics Lab, Georgetown University</t>
+  </si>
+  <si>
+    <t>Worked with Maggie Cicco on compiling special education expenditure and achievement data for selected states</t>
+  </si>
+  <si>
+    <t>Planned, organized, and advocated for teaching staff and community rights to administrators</t>
+  </si>
+  <si>
+    <t>Berkeley Initiative for Transparency in the Social Sciences (BITSS)</t>
+  </si>
+  <si>
+    <t>Research Transparency and Reproducibility Training (RT2) funding</t>
+  </si>
+  <si>
+    <t>Certificate in Education Finance</t>
+  </si>
+  <si>
+    <t>National Assessment of Educational Progress (NAEP) Data Training</t>
+  </si>
+  <si>
+    <t>Department of Education, USA</t>
+  </si>
+  <si>
+    <t>Invitation to participate in the NAEP data training organized by Department of Education and American Institute for Research (AIR) in Arlington, Virginia</t>
+  </si>
+  <si>
+    <t>Scholarship to join the 3-month certificate program on school finance with in-person sessions in Seattle, WA and virtual sessions</t>
+  </si>
+  <si>
+    <t>Invitation to participate in an training on Open-Science practices organized by University of California, Berkley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">award </t>
+  </si>
+  <si>
+    <t>Office of the Vice President for Research and Innovation, University of Oregon</t>
+  </si>
+  <si>
+    <t>Innovation Faculty Research Award</t>
+  </si>
+  <si>
+    <t>Awarded to Prof. David Liebowitz for our co-led project on school discipline</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Lorraine Moe Davis Scholarship </t>
     </r>
@@ -203,7 +282,7 @@
       <rPr>
         <sz val="10"/>
         <color indexed="8"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
       <t>and the</t>
@@ -213,90 +292,11 @@
         <b/>
         <sz val="10"/>
         <color indexed="8"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> College of Education Scholarship</t>
     </r>
-  </si>
-  <si>
-    <t>College of Education</t>
-  </si>
-  <si>
-    <t>7000</t>
-  </si>
-  <si>
-    <t>Ph.D. Quantitative Research Methods in Education</t>
-  </si>
-  <si>
-    <t>For presenting research at AEFP, Baltimore, 2023</t>
-  </si>
-  <si>
-    <t>For attending workshop on 'Big Data with Arrow in R' at PostIt, Seattle, 2024</t>
-  </si>
-  <si>
-    <t>For poster titled Who Are the Students Schools Frequently Suspend?</t>
-  </si>
-  <si>
-    <t>For poster titled Diversity, Expenditure, and Achievement in US Public Schools</t>
-  </si>
-  <si>
-    <t>Summer 2022-2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Worked with Dr. David Liebowitz on projects related to school leadership and school discipline
-</t>
-  </si>
-  <si>
-    <t>Worked with Dr. Gina Biancarosa and Dr. Patrick Kennedy on projects related to Dynamic Indicators of Basic Early Literacy Skill (DIBELS8) reading assessments</t>
-  </si>
-  <si>
-    <t>Research Contract</t>
-  </si>
-  <si>
-    <t>Edunomics Lab, Georgetown University</t>
-  </si>
-  <si>
-    <t>Worked with Maggie Cicco on compiling special education expenditure and achievement data for selected states</t>
-  </si>
-  <si>
-    <t>Planned, organized, and advocated for teaching staff and community rights to administrators</t>
-  </si>
-  <si>
-    <t>Berkeley Initiative for Transparency in the Social Sciences (BITSS)</t>
-  </si>
-  <si>
-    <t>Research Transparency and Reproducibility Training (RT2) funding</t>
-  </si>
-  <si>
-    <t>Certificate in Education Finance</t>
-  </si>
-  <si>
-    <t>National Assessment of Educational Progress (NAEP) Data Training</t>
-  </si>
-  <si>
-    <t>Department of Education, USA</t>
-  </si>
-  <si>
-    <t>Invitation to participate in the NAEP data training organized by Department of Education and American Institute for Research (AIR) in Arlington, Virginia</t>
-  </si>
-  <si>
-    <t>Scholarship to join the 3-month certificate program on school finance with in-person sessions in Seattle, WA and virtual sessions</t>
-  </si>
-  <si>
-    <t>Invitation to participate in an training on Open-Science practices organized by University of California, Berkley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">award </t>
-  </si>
-  <si>
-    <t>Office of the Vice President for Research and Innovation, University of Oregon</t>
-  </si>
-  <si>
-    <t>Innovation Faculty Research Award</t>
-  </si>
-  <si>
-    <t>Awarded to Prof. David Liebowitz for our co-led project on school discipline</t>
   </si>
 </sst>
 </file>
@@ -316,38 +316,38 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Serif"/>
-      <family val="1"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Liberation Serif"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -412,15 +412,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -428,33 +422,30 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1617,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1635,219 +1626,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>2021</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="9" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="9"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>2022</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>2014</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>2017</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>2024</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="22" t="s">
-        <v>71</v>
-      </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="2"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>2022</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="13">
+        <v>2021</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B10" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C10" s="2">
         <v>2021</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
-        <v>2019</v>
-      </c>
-      <c r="C10" s="4">
-        <v>2021</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="10" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -1856,244 +1848,248 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="10" t="s">
-        <v>72</v>
+      <c r="F12" s="8"/>
+      <c r="G12" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="10" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>62</v>
+      <c r="G14" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="8"/>
+      <c r="D15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>63</v>
+      <c r="G15" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>64</v>
+      <c r="G16" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="2">
         <v>2023</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="5">
         <v>3600</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="5" t="s">
         <v>45</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="2">
         <v>2022</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="5">
         <v>3600</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="5" t="s">
         <v>45</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="2">
         <v>2022</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>59</v>
+      <c r="E20" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="F20" s="5">
         <v>3000</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="5" t="s">
         <v>46</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="5">
         <v>2022</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="5">
         <v>300</v>
       </c>
       <c r="G21" s="5"/>
@@ -2101,142 +2097,158 @@
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="5">
         <v>2022</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="17" t="s">
-        <v>65</v>
+      <c r="G22" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="5">
         <v>2021</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="15" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5">
         <v>6000</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="2">
         <v>2017</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="8" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="13">
         <v>2024</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="13">
+        <v>700</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="13">
+        <v>2024</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="14">
-        <v>700</v>
-      </c>
-      <c r="G25" s="24" t="s">
+      <c r="E26" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="13">
+        <v>3500</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="13">
+        <v>2024</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="14">
+      <c r="B28" s="13">
         <v>2024</v>
       </c>
-      <c r="D26" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="14">
-        <v>3500</v>
-      </c>
-      <c r="G26" s="27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="14">
-        <v>2024</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="14">
-        <v>2024</v>
-      </c>
-      <c r="D28" s="20" t="s">
+      <c r="F28" s="11">
+        <v>10000</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G28" s="27" t="s">
-        <v>84</v>
-      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
working on extracting citations
</commit_message>
<xml_diff>
--- a/khurana_cv/data/cv_entries.xlsx
+++ b/khurana_cv/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDXC\University of Oregon Dropbox\Havi Khurana\Personal\Coding projects\khurana_cv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8C4843-1F61-4970-A536-CE1032271A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9B03A0-008F-4699-8146-E0912452AF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="975" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="86">
   <si>
     <t>type</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>Awarded for outstanding academic standing, diverse experience, and research potential</t>
-  </si>
-  <si>
-    <t>Awarded for highly-qualified incoming student from diverse background and experiences</t>
   </si>
   <si>
     <t>Awarded for commitment towards educational equity</t>
@@ -294,12 +291,21 @@
   <si>
     <t>short_cv</t>
   </si>
+  <si>
+    <t>Demonstrated commitment to serving others</t>
+  </si>
+  <si>
+    <t>Recruit highly qualified incoming doctoral graduate students from diverse backgrounds who enhance and advance the academic and scholarly excellence of the university</t>
+  </si>
+  <si>
+    <t>For final plots on Diversity, Expenditure, and Achievement in US Public Schools</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -345,6 +351,11 @@
       <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Source Sans Pro Reg"/>
     </font>
   </fonts>
   <fills count="3">
@@ -408,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -442,6 +453,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1604,11 +1616,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.125" style="1" customWidth="1"/>
@@ -1621,7 +1633,7 @@
     <col min="11" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1650,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
@@ -1647,10 +1659,10 @@
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1661,7 +1673,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>8</v>
@@ -1677,7 +1689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1700,7 +1712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1723,7 +1735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1737,18 +1749,18 @@
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1766,14 +1778,14 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1787,7 +1799,7 @@
         <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
@@ -1796,7 +1808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1821,7 +1833,7 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1844,7 +1856,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1862,12 +1874,12 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1892,99 +1904,101 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="14" t="s">
         <v>40</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="21" t="s">
+        <v>83</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="33.950000000000003" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -2009,7 +2023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -2034,7 +2048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -2046,7 +2060,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="5">
         <v>3000</v>
@@ -2059,7 +2073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -2071,16 +2085,18 @@
         <v>40</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="5">
         <v>300</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -2096,12 +2112,12 @@
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="10" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -2110,23 +2126,23 @@
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F21" s="5">
         <v>6000</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>45</v>
+      <c r="G21" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -2135,19 +2151,19 @@
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.95" customHeight="1">
       <c r="A23" s="13" t="s">
         <v>16</v>
       </c>
@@ -2156,21 +2172,21 @@
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" s="12">
         <v>700</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.95" customHeight="1">
       <c r="A24" s="13" t="s">
         <v>16</v>
       </c>
@@ -2179,21 +2195,21 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F24" s="12">
         <v>3500</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.95" customHeight="1">
       <c r="A25" s="13" t="s">
         <v>16</v>
       </c>
@@ -2202,37 +2218,37 @@
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.95" customHeight="1">
       <c r="A26" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="12">
         <v>2024</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26" s="11">
         <v>10000</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="20" t="s">

</xml_diff>

<commit_message>
update readme for khurana_CV
</commit_message>
<xml_diff>
--- a/khurana_cv/data/cv_entries.xlsx
+++ b/khurana_cv/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havis\University of Oregon Dropbox\Havi Khurana\Personal\Coding projects\khurana_cv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D282A1D-8B35-4C59-B329-1B51C3D06566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0558EE45-5EA0-4FBE-9CC2-9E87A0352897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
   <si>
     <t>type</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>For presenting research at AEFP, Baltimore, 2023</t>
-  </si>
-  <si>
-    <t>For attending workshop on 'Big Data with Arrow in R' at PostIt, Seattle, 2024</t>
   </si>
   <si>
     <t>For poster titled Who Are the Students Schools Frequently Suspend?</t>
@@ -311,6 +308,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>For attending workshop on 'Big Data with Arrow in R' at PostIt, Seattle, 2024 and presenting at APPAM at National Harbor, Maryland in 2024</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -1675,7 +1678,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.149999999999999" customHeight="1">
@@ -1696,7 +1699,7 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>22</v>
@@ -1723,7 +1726,7 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="4" t="s">
@@ -1748,7 +1751,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="4" t="s">
@@ -1769,11 +1772,11 @@
         <v>13</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="4" t="s">
@@ -1794,11 +1797,11 @@
         <v>13</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="4" t="s">
@@ -1894,7 +1897,7 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -1962,10 +1965,10 @@
         <v>46</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1988,7 +1991,7 @@
         <v>52</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -2002,7 +2005,7 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>53</v>
@@ -2011,7 +2014,7 @@
         <v>54</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
@@ -2111,7 +2114,7 @@
         <v>300</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -2132,7 +2135,7 @@
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2149,13 +2152,13 @@
         <v>44</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F21" s="5">
         <v>6000</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="5" t="s">
@@ -2171,10 +2174,10 @@
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
@@ -2192,16 +2195,16 @@
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" s="12">
         <v>700</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -2215,16 +2218,16 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24" s="12">
         <v>3500</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -2238,37 +2241,37 @@
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9" ht="16" customHeight="1">
       <c r="A26" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="12">
         <v>2024</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F26" s="11">
         <v>10000</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="20" t="s">

</xml_diff>